<commit_message>
Função que registra o log
</commit_message>
<xml_diff>
--- a/arquivos/Depositos por cliente.xlsx
+++ b/arquivos/Depositos por cliente.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -438,25 +438,25 @@
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C2" t="str">
-        <v>VIBRA BARUERI</v>
+        <v>VIBRA SJ DO RIO PRETO</v>
       </c>
       <c r="D2" t="str">
-        <v>0101/21I</v>
+        <v>0081/23C</v>
       </c>
       <c r="E2" t="str">
-        <v>BR - ATLANTICA BREEZE - 0,7261 - BL 02</v>
+        <v>VIBRA - STI VILLE  - BL 06 - 0,8165</v>
       </c>
       <c r="F2" t="str">
-        <v>GASOLINA A</v>
+        <v>OLEO DIESEL S500</v>
       </c>
       <c r="G2" t="str">
-        <v>ONU 1203, GASOLINA A</v>
+        <v>ONU 1202, OLEO DIESEL S500</v>
       </c>
       <c r="H2" t="str">
-        <v>142</v>
+        <v>29.271</v>
       </c>
       <c r="I2" t="str">
-        <v>114</v>
+        <v>24.002</v>
       </c>
       <c r="J2" t="str">
         <v>0</v>
@@ -471,10 +471,10 @@
         <v>0</v>
       </c>
       <c r="N2" t="str">
-        <v>142</v>
+        <v>29.271</v>
       </c>
       <c r="O2" t="str">
-        <v>114</v>
+        <v>24.002</v>
       </c>
       <c r="P2" t="str">
         <v>0</v>
@@ -488,25 +488,25 @@
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C3" t="str">
-        <v>VIBRA RIBEIRAO PRETO</v>
+        <v>VIBRA BARUERI</v>
       </c>
       <c r="D3" t="str">
-        <v>0124/23E</v>
+        <v>0102/23B</v>
       </c>
       <c r="E3" t="str">
-        <v>TRANSFER P/ VIBRA RIBEIRAO PRETO CONF NF 1262091 - 0 DE 07/07/2023</v>
+        <v>VIBRA - WECO MADELEINE - BL 2 - 0,8304</v>
       </c>
       <c r="F3" t="str">
         <v>OLEO DIESEL S10</v>
       </c>
       <c r="G3" t="str">
-        <v>OLEO DIESEL S10 ONU</v>
+        <v>ONU 1202, DIESEL S10</v>
       </c>
       <c r="H3" t="str">
-        <v>21.037</v>
+        <v>39</v>
       </c>
       <c r="I3" t="str">
-        <v>17.518</v>
+        <v>35</v>
       </c>
       <c r="J3" t="str">
         <v>0</v>
@@ -521,10 +521,10 @@
         <v>0</v>
       </c>
       <c r="N3" t="str">
-        <v>21.037</v>
+        <v>39</v>
       </c>
       <c r="O3" t="str">
-        <v>17.518</v>
+        <v>35</v>
       </c>
       <c r="P3" t="str">
         <v>0</v>
@@ -538,25 +538,25 @@
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C4" t="str">
-        <v>VIBRA PRESIDENTE PRUDENTE</v>
+        <v>VIBRA BARUERI</v>
       </c>
       <c r="D4" t="str">
-        <v>0124/23F</v>
+        <v>0278/23F</v>
       </c>
       <c r="E4" t="str">
-        <v>TRANSF VIBRA CUBATÃO CONF NFE 1264380-0 DE 18.07.2023 - DENS. 0,8314</v>
+        <v>TRANSF VIBRA.CUBATÃO X V.BARUERI CONF NF 1273775-0 29.08.23</v>
       </c>
       <c r="F4" t="str">
         <v>OLEO DIESEL S10</v>
       </c>
       <c r="G4" t="str">
-        <v>OLEO DIESEL S10 ONU</v>
+        <v>ONU 1202, DIESEL S10</v>
       </c>
       <c r="H4" t="str">
-        <v>7.647</v>
+        <v>900</v>
       </c>
       <c r="I4" t="str">
-        <v>6.358</v>
+        <v>3.489</v>
       </c>
       <c r="J4" t="str">
         <v>0</v>
@@ -571,10 +571,10 @@
         <v>0</v>
       </c>
       <c r="N4" t="str">
-        <v>7.647</v>
+        <v>900</v>
       </c>
       <c r="O4" t="str">
-        <v>6.358</v>
+        <v>3.489</v>
       </c>
       <c r="P4" t="str">
         <v>0</v>
@@ -588,25 +588,25 @@
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C5" t="str">
-        <v>VIBRA PRESIDENTE PRUDENTE</v>
+        <v>VIBRA BARUERI</v>
       </c>
       <c r="D5" t="str">
-        <v>0154/23</v>
+        <v>0283/23C</v>
       </c>
       <c r="E5" t="str">
-        <v>TRANSF PROP VIBRA PRES.PRUDENTE NF NF 3721075-1 09.08.2023 DENS 0,8314</v>
+        <v>VIBRA X VIBRA BARUERI CONF NF 1278522 20.09.23</v>
       </c>
       <c r="F5" t="str">
-        <v>OLEO DIESEL S10</v>
+        <v>OLEO DIESEL S500</v>
       </c>
       <c r="G5" t="str">
-        <v>OLEO DIESEL S10 ONU</v>
+        <v>ONU 1202, OLEO DIESEL S500</v>
       </c>
       <c r="H5" t="str">
-        <v>23.770</v>
+        <v>3.240</v>
       </c>
       <c r="I5" t="str">
-        <v>19.486</v>
+        <v>2.430</v>
       </c>
       <c r="J5" t="str">
         <v>0</v>
@@ -621,10 +621,10 @@
         <v>0</v>
       </c>
       <c r="N5" t="str">
-        <v>23.770</v>
+        <v>3.240</v>
       </c>
       <c r="O5" t="str">
-        <v>19.486</v>
+        <v>2.430</v>
       </c>
       <c r="P5" t="str">
         <v>0</v>
@@ -638,25 +638,25 @@
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C6" t="str">
-        <v>VIBRA RIBEIRAO PRETO</v>
+        <v>VIBRA SAO PAULO</v>
       </c>
       <c r="D6" t="str">
-        <v>0177/23D</v>
+        <v>0283/23D</v>
       </c>
       <c r="E6" t="str">
-        <v>TRANSF  VIBRA CUB X V.RIB.PRETO CONF NF 1283138-1 09.10.23</v>
+        <v>VIBRA CUB X V. SP CONF NF 1279755-0 25.09.23</v>
       </c>
       <c r="F6" t="str">
-        <v>OLEO DIESEL S10</v>
+        <v>OLEO DIESEL S500</v>
       </c>
       <c r="G6" t="str">
-        <v>OLEO DIESEL S10 ONU</v>
+        <v>ONU 1202, OLEO DIESEL S500</v>
       </c>
       <c r="H6" t="str">
-        <v>859</v>
+        <v>6.677</v>
       </c>
       <c r="I6" t="str">
-        <v>750</v>
+        <v>5.371</v>
       </c>
       <c r="J6" t="str">
         <v>0</v>
@@ -671,10 +671,10 @@
         <v>0</v>
       </c>
       <c r="N6" t="str">
-        <v>859</v>
+        <v>6.677</v>
       </c>
       <c r="O6" t="str">
-        <v>750</v>
+        <v>5.371</v>
       </c>
       <c r="P6" t="str">
         <v>0</v>
@@ -688,25 +688,25 @@
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C7" t="str">
-        <v>VIBRA CUBATAO</v>
+        <v>VIBRA BARUERI</v>
       </c>
       <c r="D7" t="str">
-        <v>0181/22</v>
+        <v>0283/23E</v>
       </c>
       <c r="E7" t="str">
-        <v>BR - ATLANTICA BREEZE - 0,7261 - BL 02</v>
+        <v>VIBRA SP X V. BARUERI  CONF NF 3103142-1 26.09.23</v>
       </c>
       <c r="F7" t="str">
-        <v>GASOLINA A</v>
+        <v>OLEO DIESEL S500</v>
       </c>
       <c r="G7" t="str">
-        <v>ONU 1203, GASOLINA A</v>
+        <v>ONU 1202, OLEO DIESEL S500</v>
       </c>
       <c r="H7" t="str">
-        <v>3.000</v>
+        <v>9.938</v>
       </c>
       <c r="I7" t="str">
-        <v>2.178</v>
+        <v>8.170</v>
       </c>
       <c r="J7" t="str">
         <v>0</v>
@@ -721,10 +721,10 @@
         <v>0</v>
       </c>
       <c r="N7" t="str">
-        <v>3.000</v>
+        <v>9.938</v>
       </c>
       <c r="O7" t="str">
-        <v>2.178</v>
+        <v>8.170</v>
       </c>
       <c r="P7" t="str">
         <v>0</v>
@@ -738,13 +738,13 @@
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C8" t="str">
-        <v>VIBRA PAULINIA</v>
+        <v>VIBRA CUBATAO</v>
       </c>
       <c r="D8" t="str">
-        <v>0192/23B</v>
+        <v>0283/23G</v>
       </c>
       <c r="E8" t="str">
-        <v>TRANSF V.CUB X PAULINIA CONF NF 1285075-0 DENS:0,8298</v>
+        <v>TRANSF VIBRA PAU X  VIBRA CUB CONF NF 3749230-0 04.10.23</v>
       </c>
       <c r="F8" t="str">
         <v>OLEO DIESEL S500</v>
@@ -753,10 +753,10 @@
         <v>ONU 1202, OLEO DIESEL S500</v>
       </c>
       <c r="H8" t="str">
-        <v>3.902</v>
+        <v>86</v>
       </c>
       <c r="I8" t="str">
-        <v>7.967</v>
+        <v>4.190</v>
       </c>
       <c r="J8" t="str">
         <v>0</v>
@@ -771,10 +771,10 @@
         <v>0</v>
       </c>
       <c r="N8" t="str">
-        <v>3.902</v>
+        <v>86</v>
       </c>
       <c r="O8" t="str">
-        <v>7.967</v>
+        <v>4.190</v>
       </c>
       <c r="P8" t="str">
         <v>0</v>
@@ -782,31 +782,31 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>TQ-17</v>
+        <v>QUEBRA</v>
       </c>
       <c r="B9" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C9" t="str">
-        <v>VIBRA CUBATAO</v>
+        <v>VIBRA RIBEIRAO PRETO</v>
       </c>
       <c r="D9" t="str">
-        <v>0177/23B</v>
+        <v>0283/23H</v>
       </c>
       <c r="E9" t="str">
-        <v>TRANSF NIMOFAST X VIBRA CUB CONF NF 2217-1 09.10.23</v>
+        <v>VIBRA - AQUARIUS - NF 1272825 DENSIDADE 0,8290</v>
       </c>
       <c r="F9" t="str">
-        <v>OLEO DIESEL S10</v>
+        <v>OLEO DIESEL S500</v>
       </c>
       <c r="G9" t="str">
-        <v>OLEO DIESEL S10 ONU</v>
+        <v>ONU 1202, OLEO DIESEL S500</v>
       </c>
       <c r="H9" t="str">
-        <v>951</v>
+        <v>16.640</v>
       </c>
       <c r="I9" t="str">
-        <v>764</v>
+        <v>13.385</v>
       </c>
       <c r="J9" t="str">
         <v>0</v>
@@ -821,10 +821,10 @@
         <v>0</v>
       </c>
       <c r="N9" t="str">
-        <v>951</v>
+        <v>16.640</v>
       </c>
       <c r="O9" t="str">
-        <v>764</v>
+        <v>13.385</v>
       </c>
       <c r="P9" t="str">
         <v>0</v>
@@ -832,19 +832,19 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>TQ-23</v>
+        <v>QUEBRA</v>
       </c>
       <c r="B10" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C10" t="str">
-        <v>VIBRA SJ CAMPOS</v>
+        <v>VIBRA CUBATAO</v>
       </c>
       <c r="D10" t="str">
-        <v>0053/22E</v>
+        <v>0283/23I</v>
       </c>
       <c r="E10" t="str">
-        <v>VIBRA - RIDGEBURY CINDY A - BL RBYK23546293 - 0,8287</v>
+        <v>TRANSF VIBRA PAULINIA CONF NF 3749795-1 05.09.23</v>
       </c>
       <c r="F10" t="str">
         <v>OLEO DIESEL S500</v>
@@ -853,10 +853,10 @@
         <v>ONU 1202, OLEO DIESEL S500</v>
       </c>
       <c r="H10" t="str">
-        <v>604</v>
+        <v>12.421</v>
       </c>
       <c r="I10" t="str">
-        <v>501</v>
+        <v>6.166</v>
       </c>
       <c r="J10" t="str">
         <v>0</v>
@@ -871,10 +871,10 @@
         <v>0</v>
       </c>
       <c r="N10" t="str">
-        <v>604</v>
+        <v>12.421</v>
       </c>
       <c r="O10" t="str">
-        <v>501</v>
+        <v>6.166</v>
       </c>
       <c r="P10" t="str">
         <v>0</v>
@@ -882,31 +882,31 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>TQ-23</v>
+        <v>QUEBRA</v>
       </c>
       <c r="B11" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C11" t="str">
-        <v>VIBRA SAO PAULO</v>
+        <v>VIBRA RIBEIRAO PRETO</v>
       </c>
       <c r="D11" t="str">
-        <v>0113/22I</v>
+        <v>0307/23J</v>
       </c>
       <c r="E11" t="str">
-        <v>VIBRA - ZANDOLIE - BL 6 - 0,8380</v>
+        <v>TRANSF VIBRA CUB X V.RIB PRETO CONF NF 1281710 - 0 03.10.23</v>
       </c>
       <c r="F11" t="str">
-        <v>OLEO DIESEL S500</v>
+        <v>OLEO DIESEL S10</v>
       </c>
       <c r="G11" t="str">
-        <v>ONU 1202, OLEO DIESEL S500</v>
+        <v>ONU 1202, DIESEL S10</v>
       </c>
       <c r="H11" t="str">
-        <v>235</v>
+        <v>8.967</v>
       </c>
       <c r="I11" t="str">
-        <v>0</v>
+        <v>8.257</v>
       </c>
       <c r="J11" t="str">
         <v>0</v>
@@ -921,10 +921,10 @@
         <v>0</v>
       </c>
       <c r="N11" t="str">
-        <v>235</v>
+        <v>8.967</v>
       </c>
       <c r="O11" t="str">
-        <v>0</v>
+        <v>8.257</v>
       </c>
       <c r="P11" t="str">
         <v>0</v>
@@ -932,31 +932,31 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>TQ-23</v>
+        <v>QUEBRA</v>
       </c>
       <c r="B12" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C12" t="str">
-        <v>VIBRA RIBEIRAO PRETO</v>
+        <v>VIBRA SAO PAULO</v>
       </c>
       <c r="D12" t="str">
-        <v>0192/23D</v>
+        <v>0307/23M</v>
       </c>
       <c r="E12" t="str">
-        <v>TRANSF V.CUB X R.PRETO CONF NF 12470085-0 DENS:0,8298</v>
+        <v>TRANSF  VIBRA PAU CONF NF 3750527-1 06.10.23</v>
       </c>
       <c r="F12" t="str">
-        <v>OLEO DIESEL S500</v>
+        <v>OLEO DIESEL S10</v>
       </c>
       <c r="G12" t="str">
-        <v>ONU 1202, OLEO DIESEL S500</v>
+        <v>ONU 1202, DIESEL S10</v>
       </c>
       <c r="H12" t="str">
-        <v>22.000</v>
+        <v>34.074</v>
       </c>
       <c r="I12" t="str">
-        <v>18.408</v>
+        <v>28.080</v>
       </c>
       <c r="J12" t="str">
         <v>0</v>
@@ -971,10 +971,10 @@
         <v>0</v>
       </c>
       <c r="N12" t="str">
-        <v>22.000</v>
+        <v>34.074</v>
       </c>
       <c r="O12" t="str">
-        <v>18.408</v>
+        <v>28.080</v>
       </c>
       <c r="P12" t="str">
         <v>0</v>
@@ -982,31 +982,31 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>TQ-38</v>
+        <v>TQ-03</v>
       </c>
       <c r="B13" t="str">
-        <v>IMPORTACAO COMUM</v>
+        <v>MERCADO INTERNO</v>
       </c>
       <c r="C13" t="str">
-        <v>VIBRA CUBATAO</v>
+        <v>VIBRA PAULINIA</v>
       </c>
       <c r="D13" t="str">
-        <v>0192/23A</v>
+        <v>0174/23Z</v>
       </c>
       <c r="E13" t="str">
-        <v>TORM ATLANTIC - VIBRA CUBATÃO BL:05 - DENS:0,8305</v>
+        <v>TRANSF VIBRA CUBATÃO CONF NFE 1264138-0 DE 17.07.2023</v>
       </c>
       <c r="F13" t="str">
-        <v>OLEO DIESEL S500</v>
+        <v>OLEO DIESEL S10</v>
       </c>
       <c r="G13" t="str">
-        <v>ONU 1202, OLEO DIESEL S500</v>
+        <v>ONU 1202, DIESEL S10</v>
       </c>
       <c r="H13" t="str">
-        <v>1.805</v>
+        <v>73</v>
       </c>
       <c r="I13" t="str">
-        <v>2.000</v>
+        <v>62</v>
       </c>
       <c r="J13" t="str">
         <v>0</v>
@@ -1021,10 +1021,10 @@
         <v>0</v>
       </c>
       <c r="N13" t="str">
-        <v>1.805</v>
+        <v>73</v>
       </c>
       <c r="O13" t="str">
-        <v>2.000</v>
+        <v>62</v>
       </c>
       <c r="P13" t="str">
         <v>0</v>
@@ -1032,31 +1032,31 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>TQ-38</v>
+        <v>TQ-03</v>
       </c>
       <c r="B14" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C14" t="str">
-        <v>VIBRA SAO PAULO</v>
+        <v>VIBRA PRESIDENTE PRUDENTE</v>
       </c>
       <c r="D14" t="str">
-        <v>0192/23C</v>
+        <v>0259/23G</v>
       </c>
       <c r="E14" t="str">
-        <v>TRANSF V.CUB X SP CONF NF 1285073-0 DENS:0,8298</v>
+        <v>TRANSF VIBRA CUB X PRE.PRUDENTE CONF NF 1276885-0 12.09.2023</v>
       </c>
       <c r="F14" t="str">
-        <v>OLEO DIESEL S500</v>
+        <v>OLEO DIESEL S10</v>
       </c>
       <c r="G14" t="str">
-        <v>ONU 1202, OLEO DIESEL S500</v>
+        <v>ONU 1202, DIESEL S10</v>
       </c>
       <c r="H14" t="str">
-        <v>22.696</v>
+        <v>13.503</v>
       </c>
       <c r="I14" t="str">
-        <v>18.460</v>
+        <v>11.526</v>
       </c>
       <c r="J14" t="str">
         <v>0</v>
@@ -1071,10 +1071,10 @@
         <v>0</v>
       </c>
       <c r="N14" t="str">
-        <v>22.696</v>
+        <v>13.503</v>
       </c>
       <c r="O14" t="str">
-        <v>18.460</v>
+        <v>11.526</v>
       </c>
       <c r="P14" t="str">
         <v>0</v>
@@ -1082,31 +1082,31 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>TQ-38</v>
+        <v>TQ-03</v>
       </c>
       <c r="B15" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C15" t="str">
-        <v>VIBRA RIBEIRAO PRETO</v>
+        <v>VIBRA PAULINIA</v>
       </c>
       <c r="D15" t="str">
-        <v>0192/23D</v>
+        <v>0307/23L</v>
       </c>
       <c r="E15" t="str">
-        <v>TRANSF V.CUB X R.PRETO CONF NF 12470085-0 DENS:0,8298</v>
+        <v>TRANSF  VIBRA CUB CONF NF1282508 1 06.10.23</v>
       </c>
       <c r="F15" t="str">
-        <v>OLEO DIESEL S500</v>
+        <v>OLEO DIESEL S10</v>
       </c>
       <c r="G15" t="str">
-        <v>ONU 1202, OLEO DIESEL S500</v>
+        <v>ONU 1202, DIESEL S10</v>
       </c>
       <c r="H15" t="str">
-        <v>467.996</v>
+        <v>45.628</v>
       </c>
       <c r="I15" t="str">
-        <v>388.098</v>
+        <v>38.507</v>
       </c>
       <c r="J15" t="str">
         <v>0</v>
@@ -1121,10 +1121,10 @@
         <v>0</v>
       </c>
       <c r="N15" t="str">
-        <v>467.996</v>
+        <v>45.628</v>
       </c>
       <c r="O15" t="str">
-        <v>388.098</v>
+        <v>38.507</v>
       </c>
       <c r="P15" t="str">
         <v>0</v>
@@ -1132,31 +1132,31 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>TQ-38</v>
+        <v>TQ-03</v>
       </c>
       <c r="B16" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C16" t="str">
-        <v>VIBRA CUBATAO</v>
+        <v>VIBRA SAO PAULO</v>
       </c>
       <c r="D16" t="str">
-        <v>0192/23E</v>
+        <v>0307/23M</v>
       </c>
       <c r="E16" t="str">
-        <v>TRANSF PAULINIA-CUBATAO CONF NF 3749230-1 DENS:0,8298</v>
+        <v>TRANSF  VIBRA PAU CONF NF 3750527-1 06.10.23</v>
       </c>
       <c r="F16" t="str">
-        <v>OLEO DIESEL S500</v>
+        <v>OLEO DIESEL S10</v>
       </c>
       <c r="G16" t="str">
-        <v>ONU 1202, OLEO DIESEL S500</v>
+        <v>ONU 1202, DIESEL S10</v>
       </c>
       <c r="H16" t="str">
-        <v>10.112</v>
+        <v>72.525</v>
       </c>
       <c r="I16" t="str">
-        <v>9.685</v>
+        <v>60.000</v>
       </c>
       <c r="J16" t="str">
         <v>0</v>
@@ -1171,10 +1171,10 @@
         <v>0</v>
       </c>
       <c r="N16" t="str">
-        <v>10.112</v>
+        <v>72.525</v>
       </c>
       <c r="O16" t="str">
-        <v>9.685</v>
+        <v>60.000</v>
       </c>
       <c r="P16" t="str">
         <v>0</v>
@@ -1182,19 +1182,19 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>TQ-68</v>
+        <v>TQ-03</v>
       </c>
       <c r="B17" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C17" t="str">
-        <v>VIBRA PRESIDENTE PRUDENTE</v>
+        <v>VIBRA PAULINIA</v>
       </c>
       <c r="D17" t="str">
-        <v>0169/23F</v>
+        <v>0307/23N</v>
       </c>
       <c r="E17" t="str">
-        <v>VIBRA CUB TRANSF CONF NF 1277460-0 14.09.23</v>
+        <v>AJUSTE DE SALDO (CONF NF 3759087-1 24.10.23)</v>
       </c>
       <c r="F17" t="str">
         <v>OLEO DIESEL S10</v>
@@ -1203,10 +1203,10 @@
         <v>ONU 1202, DIESEL S10</v>
       </c>
       <c r="H17" t="str">
-        <v>1.643</v>
+        <v>8.052</v>
       </c>
       <c r="I17" t="str">
-        <v>2.980</v>
+        <v>6.764</v>
       </c>
       <c r="J17" t="str">
         <v>0</v>
@@ -1221,10 +1221,10 @@
         <v>0</v>
       </c>
       <c r="N17" t="str">
-        <v>1.643</v>
+        <v>8.052</v>
       </c>
       <c r="O17" t="str">
-        <v>2.980</v>
+        <v>6.764</v>
       </c>
       <c r="P17" t="str">
         <v>0</v>
@@ -1232,19 +1232,19 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>TQ-68</v>
+        <v>TQ-03</v>
       </c>
       <c r="B18" t="str">
-        <v>MERCADO INTERNO</v>
+        <v>IMPORTACAO COMUM</v>
       </c>
       <c r="C18" t="str">
         <v>VIBRA CUBATAO</v>
       </c>
       <c r="D18" t="str">
-        <v>0169/23G</v>
+        <v>0322/23A</v>
       </c>
       <c r="E18" t="str">
-        <v>VIBRA PRES TRANSF CONF NF 607274-0 26.09.2023</v>
+        <v>TORM ALTLANTIC - VIBRA CUBATÃO - BL 02 DENS:0,8306</v>
       </c>
       <c r="F18" t="str">
         <v>OLEO DIESEL S10</v>
@@ -1253,10 +1253,10 @@
         <v>ONU 1202, DIESEL S10</v>
       </c>
       <c r="H18" t="str">
-        <v>20.556</v>
+        <v>21.161</v>
       </c>
       <c r="I18" t="str">
-        <v>17.730</v>
+        <v>3.597</v>
       </c>
       <c r="J18" t="str">
         <v>0</v>
@@ -1271,10 +1271,10 @@
         <v>0</v>
       </c>
       <c r="N18" t="str">
-        <v>20.556</v>
+        <v>21.161</v>
       </c>
       <c r="O18" t="str">
-        <v>17.730</v>
+        <v>3.597</v>
       </c>
       <c r="P18" t="str">
         <v>0</v>
@@ -1282,49 +1282,49 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>TQ-68</v>
+        <v>TQ-03</v>
       </c>
       <c r="B19" t="str">
-        <v>MERCADO INTERNO</v>
+        <v>IMPORTACAO COMUM</v>
       </c>
       <c r="C19" t="str">
         <v>VIBRA CUBATAO</v>
       </c>
       <c r="D19" t="str">
-        <v>0177/23B</v>
+        <v>0322/23B</v>
       </c>
       <c r="E19" t="str">
-        <v>TRANSF NIMOFAST X VIBRA CUB CONF NF 2217-1 09.10.23</v>
+        <v>TORM ALTLANTIC - VIBRA CUBATÃO - BL 08 DENS: FALTA</v>
       </c>
       <c r="F19" t="str">
         <v>OLEO DIESEL S10</v>
       </c>
       <c r="G19" t="str">
-        <v>OLEO DIESEL S10 ONU</v>
+        <v>ONU 1202, DIESEL S10</v>
       </c>
       <c r="H19" t="str">
-        <v>2.200</v>
+        <v>0</v>
       </c>
       <c r="I19" t="str">
-        <v>1.145</v>
+        <v>0</v>
       </c>
       <c r="J19" t="str">
         <v>0</v>
       </c>
       <c r="K19" t="str">
-        <v>0</v>
+        <v>5.006.360</v>
       </c>
       <c r="L19" t="str">
-        <v>0</v>
+        <v>4.158.176</v>
       </c>
       <c r="M19" t="str">
         <v>0</v>
       </c>
       <c r="N19" t="str">
-        <v>2.200</v>
+        <v>5.006.360</v>
       </c>
       <c r="O19" t="str">
-        <v>1.145</v>
+        <v>4.158.176</v>
       </c>
       <c r="P19" t="str">
         <v>0</v>
@@ -1332,7 +1332,7 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>TQ-68</v>
+        <v>TQ-03</v>
       </c>
       <c r="B20" t="str">
         <v>MERCADO INTERNO</v>
@@ -1341,22 +1341,22 @@
         <v>VIBRA PAULINIA</v>
       </c>
       <c r="D20" t="str">
-        <v>0177/23C</v>
+        <v>0322/23C</v>
       </c>
       <c r="E20" t="str">
-        <v>TRANSF  VIBRA CUB P/VIBRA PAULINIA CONF NF 1283140-0 DE09.10.23</v>
+        <v>TRANSF VIBRA CUB X PAULINIA CONF NF 1286527-0 25.10.23</v>
       </c>
       <c r="F20" t="str">
         <v>OLEO DIESEL S10</v>
       </c>
       <c r="G20" t="str">
-        <v>OLEO DIESEL S10 ONU</v>
+        <v>ONU 1202, DIESEL S10</v>
       </c>
       <c r="H20" t="str">
-        <v>10.136</v>
+        <v>186.385</v>
       </c>
       <c r="I20" t="str">
-        <v>10.110</v>
+        <v>154.810</v>
       </c>
       <c r="J20" t="str">
         <v>0</v>
@@ -1371,10 +1371,10 @@
         <v>0</v>
       </c>
       <c r="N20" t="str">
-        <v>10.136</v>
+        <v>186.385</v>
       </c>
       <c r="O20" t="str">
-        <v>10.110</v>
+        <v>154.810</v>
       </c>
       <c r="P20" t="str">
         <v>0</v>
@@ -1382,31 +1382,31 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>TQ-68</v>
+        <v>TQ-03</v>
       </c>
       <c r="B21" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C21" t="str">
-        <v>VIBRA BARUERI</v>
+        <v>VIBRA PRESIDENTE PRUDENTE</v>
       </c>
       <c r="D21" t="str">
-        <v>0177/23E</v>
+        <v>0322/23D</v>
       </c>
       <c r="E21" t="str">
-        <v>TRANSF  VIBRA CUB X VIBRA BARUERI CONF NF 1283141 09.10.23</v>
+        <v>TORM ALTLANTIC - VIBRA CUBATÃO - BL 02 DENS:0,8306</v>
       </c>
       <c r="F21" t="str">
         <v>OLEO DIESEL S10</v>
       </c>
       <c r="G21" t="str">
-        <v>OLEO DIESEL S10 ONU</v>
+        <v>ONU 1202, DIESEL S10</v>
       </c>
       <c r="H21" t="str">
-        <v>904.342</v>
+        <v>5.000.000</v>
       </c>
       <c r="I21" t="str">
-        <v>748.400</v>
+        <v>4.166.500</v>
       </c>
       <c r="J21" t="str">
         <v>0</v>
@@ -1421,10 +1421,10 @@
         <v>0</v>
       </c>
       <c r="N21" t="str">
-        <v>904.342</v>
+        <v>5.000.000</v>
       </c>
       <c r="O21" t="str">
-        <v>748.400</v>
+        <v>4.166.500</v>
       </c>
       <c r="P21" t="str">
         <v>0</v>
@@ -1432,42 +1432,142 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
+        <v>TQ-07</v>
+      </c>
+      <c r="B22" t="str">
+        <v>IMPORTACAO COMUM</v>
+      </c>
+      <c r="C22" t="str">
+        <v>VIBRA CUBATAO</v>
+      </c>
+      <c r="D22" t="str">
+        <v>0322/23</v>
+      </c>
+      <c r="E22" t="str">
+        <v>TORM ALTLANTIC - VIBRA CUBATÃO - BL 01 DENS: 0,8306</v>
+      </c>
+      <c r="F22" t="str">
+        <v>OLEO DIESEL S10</v>
+      </c>
+      <c r="G22" t="str">
+        <v>ONU 1202, DIESEL S10</v>
+      </c>
+      <c r="H22" t="str">
+        <v>722</v>
+      </c>
+      <c r="I22" t="str">
+        <v>598</v>
+      </c>
+      <c r="J22" t="str">
+        <v>0</v>
+      </c>
+      <c r="K22" t="str">
+        <v>0</v>
+      </c>
+      <c r="L22" t="str">
+        <v>0</v>
+      </c>
+      <c r="M22" t="str">
+        <v>0</v>
+      </c>
+      <c r="N22" t="str">
+        <v>722</v>
+      </c>
+      <c r="O22" t="str">
+        <v>598</v>
+      </c>
+      <c r="P22" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>TQ-07</v>
+      </c>
+      <c r="B23" t="str">
+        <v>IMPORTACAO COMUM</v>
+      </c>
+      <c r="C23" t="str">
+        <v>VIBRA CUBATAO</v>
+      </c>
+      <c r="D23" t="str">
+        <v>0322/23A</v>
+      </c>
+      <c r="E23" t="str">
+        <v>TORM ALTLANTIC - VIBRA CUBATÃO - BL 02 DENS:0,8306</v>
+      </c>
+      <c r="F23" t="str">
+        <v>OLEO DIESEL S10</v>
+      </c>
+      <c r="G23" t="str">
+        <v>ONU 1202, DIESEL S10</v>
+      </c>
+      <c r="H23" t="str">
+        <v>4.191.190</v>
+      </c>
+      <c r="I23" t="str">
+        <v>3.481.102</v>
+      </c>
+      <c r="J23" t="str">
+        <v>0</v>
+      </c>
+      <c r="K23" t="str">
+        <v>0</v>
+      </c>
+      <c r="L23" t="str">
+        <v>0</v>
+      </c>
+      <c r="M23" t="str">
+        <v>0</v>
+      </c>
+      <c r="N23" t="str">
+        <v>4.191.190</v>
+      </c>
+      <c r="O23" t="str">
+        <v>3.481.102</v>
+      </c>
+      <c r="P23" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
         <v>Z</v>
       </c>
-      <c r="D22" t="str">
+      <c r="D24" t="str">
         <v>Total</v>
       </c>
-      <c r="H22" t="str">
-        <v>1.525.633</v>
-      </c>
-      <c r="I22" t="str">
-        <v>1.272.652</v>
-      </c>
-      <c r="J22" t="str">
-        <v>0</v>
-      </c>
-      <c r="K22" t="str">
-        <v>0</v>
-      </c>
-      <c r="L22" t="str">
-        <v>0</v>
-      </c>
-      <c r="M22" t="str">
-        <v>0</v>
-      </c>
-      <c r="N22" t="str">
-        <v>1.525.633</v>
-      </c>
-      <c r="O22" t="str">
-        <v>1.272.652</v>
-      </c>
-      <c r="P22" t="str">
+      <c r="H24" t="str">
+        <v>9.661.492</v>
+      </c>
+      <c r="I24" t="str">
+        <v>8.027.041</v>
+      </c>
+      <c r="J24" t="str">
+        <v>0</v>
+      </c>
+      <c r="K24" t="str">
+        <v>5.006.360</v>
+      </c>
+      <c r="L24" t="str">
+        <v>4.158.176</v>
+      </c>
+      <c r="M24" t="str">
+        <v>0</v>
+      </c>
+      <c r="N24" t="str">
+        <v>14.667.852</v>
+      </c>
+      <c r="O24" t="str">
+        <v>12.185.217</v>
+      </c>
+      <c r="P24" t="str">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:P22"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:P24"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
acrescentado api de registro de log sql server
</commit_message>
<xml_diff>
--- a/arquivos/Depositos por cliente.xlsx
+++ b/arquivos/Depositos por cliente.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -788,25 +788,25 @@
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C9" t="str">
-        <v>VIBRA CUBATAO</v>
+        <v>VIBRA PRESIDENTE PRUDENTE</v>
       </c>
       <c r="D9" t="str">
-        <v>0177/23B</v>
+        <v>0169/23F</v>
       </c>
       <c r="E9" t="str">
-        <v>TRANSF NIMOFAST X VIBRA CUB CONF NF 2217-1 09.10.23</v>
+        <v>VIBRA CUB TRANSF CONF NF 1277460-0 14.09.23</v>
       </c>
       <c r="F9" t="str">
         <v>OLEO DIESEL S10</v>
       </c>
       <c r="G9" t="str">
-        <v>OLEO DIESEL S10 ONU</v>
+        <v>ONU 1202, DIESEL S10</v>
       </c>
       <c r="H9" t="str">
-        <v>951</v>
+        <v>1.643</v>
       </c>
       <c r="I9" t="str">
-        <v>764</v>
+        <v>2.980</v>
       </c>
       <c r="J9" t="str">
         <v>0</v>
@@ -821,10 +821,10 @@
         <v>0</v>
       </c>
       <c r="N9" t="str">
-        <v>951</v>
+        <v>1.643</v>
       </c>
       <c r="O9" t="str">
-        <v>764</v>
+        <v>2.980</v>
       </c>
       <c r="P9" t="str">
         <v>0</v>
@@ -832,31 +832,31 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>TQ-23</v>
+        <v>TQ-17</v>
       </c>
       <c r="B10" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C10" t="str">
-        <v>VIBRA SJ CAMPOS</v>
+        <v>VIBRA CUBATAO</v>
       </c>
       <c r="D10" t="str">
-        <v>0053/22E</v>
+        <v>0169/23G</v>
       </c>
       <c r="E10" t="str">
-        <v>VIBRA - RIDGEBURY CINDY A - BL RBYK23546293 - 0,8287</v>
+        <v>VIBRA PRES TRANSF CONF NF 607274-0 26.09.2023</v>
       </c>
       <c r="F10" t="str">
-        <v>OLEO DIESEL S500</v>
+        <v>OLEO DIESEL S10</v>
       </c>
       <c r="G10" t="str">
-        <v>ONU 1202, OLEO DIESEL S500</v>
+        <v>ONU 1202, DIESEL S10</v>
       </c>
       <c r="H10" t="str">
-        <v>604</v>
+        <v>20.556</v>
       </c>
       <c r="I10" t="str">
-        <v>501</v>
+        <v>17.730</v>
       </c>
       <c r="J10" t="str">
         <v>0</v>
@@ -871,10 +871,10 @@
         <v>0</v>
       </c>
       <c r="N10" t="str">
-        <v>604</v>
+        <v>20.556</v>
       </c>
       <c r="O10" t="str">
-        <v>501</v>
+        <v>17.730</v>
       </c>
       <c r="P10" t="str">
         <v>0</v>
@@ -882,31 +882,31 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>TQ-23</v>
+        <v>TQ-17</v>
       </c>
       <c r="B11" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C11" t="str">
-        <v>VIBRA SAO PAULO</v>
+        <v>VIBRA CUBATAO</v>
       </c>
       <c r="D11" t="str">
-        <v>0113/22I</v>
+        <v>0177/23B</v>
       </c>
       <c r="E11" t="str">
-        <v>VIBRA - ZANDOLIE - BL 6 - 0,8380</v>
+        <v>TRANSF NIMOFAST X VIBRA CUB CONF NF 2217-1 09.10.23</v>
       </c>
       <c r="F11" t="str">
-        <v>OLEO DIESEL S500</v>
+        <v>OLEO DIESEL S10</v>
       </c>
       <c r="G11" t="str">
-        <v>ONU 1202, OLEO DIESEL S500</v>
+        <v>OLEO DIESEL S10 ONU</v>
       </c>
       <c r="H11" t="str">
-        <v>235</v>
+        <v>3.151</v>
       </c>
       <c r="I11" t="str">
-        <v>0</v>
+        <v>1.909</v>
       </c>
       <c r="J11" t="str">
         <v>0</v>
@@ -921,10 +921,10 @@
         <v>0</v>
       </c>
       <c r="N11" t="str">
-        <v>235</v>
+        <v>3.151</v>
       </c>
       <c r="O11" t="str">
-        <v>0</v>
+        <v>1.909</v>
       </c>
       <c r="P11" t="str">
         <v>0</v>
@@ -932,31 +932,31 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>TQ-23</v>
+        <v>TQ-17</v>
       </c>
       <c r="B12" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C12" t="str">
-        <v>VIBRA RIBEIRAO PRETO</v>
+        <v>VIBRA PAULINIA</v>
       </c>
       <c r="D12" t="str">
-        <v>0192/23D</v>
+        <v>0177/23C</v>
       </c>
       <c r="E12" t="str">
-        <v>TRANSF V.CUB X R.PRETO CONF NF 12470085-0 DENS:0,8298</v>
+        <v>TRANSF  VIBRA CUB P/VIBRA PAULINIA CONF NF 1283140-0 DE09.10.23</v>
       </c>
       <c r="F12" t="str">
-        <v>OLEO DIESEL S500</v>
+        <v>OLEO DIESEL S10</v>
       </c>
       <c r="G12" t="str">
-        <v>ONU 1202, OLEO DIESEL S500</v>
+        <v>OLEO DIESEL S10 ONU</v>
       </c>
       <c r="H12" t="str">
-        <v>22.000</v>
+        <v>10.136</v>
       </c>
       <c r="I12" t="str">
-        <v>18.408</v>
+        <v>10.110</v>
       </c>
       <c r="J12" t="str">
         <v>0</v>
@@ -971,10 +971,10 @@
         <v>0</v>
       </c>
       <c r="N12" t="str">
-        <v>22.000</v>
+        <v>10.136</v>
       </c>
       <c r="O12" t="str">
-        <v>18.408</v>
+        <v>10.110</v>
       </c>
       <c r="P12" t="str">
         <v>0</v>
@@ -982,31 +982,31 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>TQ-38</v>
+        <v>TQ-17</v>
       </c>
       <c r="B13" t="str">
-        <v>IMPORTACAO COMUM</v>
+        <v>MERCADO INTERNO</v>
       </c>
       <c r="C13" t="str">
-        <v>VIBRA CUBATAO</v>
+        <v>VIBRA BARUERI</v>
       </c>
       <c r="D13" t="str">
-        <v>0192/23A</v>
+        <v>0177/23E</v>
       </c>
       <c r="E13" t="str">
-        <v>TORM ATLANTIC - VIBRA CUBATÃO BL:05 - DENS:0,8305</v>
+        <v>TRANSF  VIBRA CUB X VIBRA BARUERI CONF NF 1283141 09.10.23</v>
       </c>
       <c r="F13" t="str">
-        <v>OLEO DIESEL S500</v>
+        <v>OLEO DIESEL S10</v>
       </c>
       <c r="G13" t="str">
-        <v>ONU 1202, OLEO DIESEL S500</v>
+        <v>OLEO DIESEL S10 ONU</v>
       </c>
       <c r="H13" t="str">
-        <v>1.805</v>
+        <v>30.435</v>
       </c>
       <c r="I13" t="str">
-        <v>2.000</v>
+        <v>25.090</v>
       </c>
       <c r="J13" t="str">
         <v>0</v>
@@ -1021,10 +1021,10 @@
         <v>0</v>
       </c>
       <c r="N13" t="str">
-        <v>1.805</v>
+        <v>30.435</v>
       </c>
       <c r="O13" t="str">
-        <v>2.000</v>
+        <v>25.090</v>
       </c>
       <c r="P13" t="str">
         <v>0</v>
@@ -1032,19 +1032,19 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>TQ-38</v>
+        <v>TQ-23</v>
       </c>
       <c r="B14" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C14" t="str">
-        <v>VIBRA SAO PAULO</v>
+        <v>VIBRA SJ CAMPOS</v>
       </c>
       <c r="D14" t="str">
-        <v>0192/23C</v>
+        <v>0053/22E</v>
       </c>
       <c r="E14" t="str">
-        <v>TRANSF V.CUB X SP CONF NF 1285073-0 DENS:0,8298</v>
+        <v>VIBRA - RIDGEBURY CINDY A - BL RBYK23546293 - 0,8287</v>
       </c>
       <c r="F14" t="str">
         <v>OLEO DIESEL S500</v>
@@ -1053,10 +1053,10 @@
         <v>ONU 1202, OLEO DIESEL S500</v>
       </c>
       <c r="H14" t="str">
-        <v>22.696</v>
+        <v>604</v>
       </c>
       <c r="I14" t="str">
-        <v>18.460</v>
+        <v>501</v>
       </c>
       <c r="J14" t="str">
         <v>0</v>
@@ -1071,10 +1071,10 @@
         <v>0</v>
       </c>
       <c r="N14" t="str">
-        <v>22.696</v>
+        <v>604</v>
       </c>
       <c r="O14" t="str">
-        <v>18.460</v>
+        <v>501</v>
       </c>
       <c r="P14" t="str">
         <v>0</v>
@@ -1082,19 +1082,19 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>TQ-38</v>
+        <v>TQ-23</v>
       </c>
       <c r="B15" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C15" t="str">
-        <v>VIBRA RIBEIRAO PRETO</v>
+        <v>VIBRA SAO PAULO</v>
       </c>
       <c r="D15" t="str">
-        <v>0192/23D</v>
+        <v>0113/22I</v>
       </c>
       <c r="E15" t="str">
-        <v>TRANSF V.CUB X R.PRETO CONF NF 12470085-0 DENS:0,8298</v>
+        <v>VIBRA - ZANDOLIE - BL 6 - 0,8380</v>
       </c>
       <c r="F15" t="str">
         <v>OLEO DIESEL S500</v>
@@ -1103,10 +1103,10 @@
         <v>ONU 1202, OLEO DIESEL S500</v>
       </c>
       <c r="H15" t="str">
-        <v>467.996</v>
+        <v>235</v>
       </c>
       <c r="I15" t="str">
-        <v>388.098</v>
+        <v>0</v>
       </c>
       <c r="J15" t="str">
         <v>0</v>
@@ -1121,10 +1121,10 @@
         <v>0</v>
       </c>
       <c r="N15" t="str">
-        <v>467.996</v>
+        <v>235</v>
       </c>
       <c r="O15" t="str">
-        <v>388.098</v>
+        <v>0</v>
       </c>
       <c r="P15" t="str">
         <v>0</v>
@@ -1132,19 +1132,19 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>TQ-38</v>
+        <v>TQ-23</v>
       </c>
       <c r="B16" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C16" t="str">
-        <v>VIBRA CUBATAO</v>
+        <v>VIBRA RIBEIRAO PRETO</v>
       </c>
       <c r="D16" t="str">
-        <v>0192/23E</v>
+        <v>0192/23D</v>
       </c>
       <c r="E16" t="str">
-        <v>TRANSF PAULINIA-CUBATAO CONF NF 3749230-1 DENS:0,8298</v>
+        <v>TRANSF V.CUB X R.PRETO CONF NF 12470085-0 DENS:0,8298</v>
       </c>
       <c r="F16" t="str">
         <v>OLEO DIESEL S500</v>
@@ -1153,10 +1153,10 @@
         <v>ONU 1202, OLEO DIESEL S500</v>
       </c>
       <c r="H16" t="str">
-        <v>10.112</v>
+        <v>22.000</v>
       </c>
       <c r="I16" t="str">
-        <v>9.685</v>
+        <v>18.408</v>
       </c>
       <c r="J16" t="str">
         <v>0</v>
@@ -1171,10 +1171,10 @@
         <v>0</v>
       </c>
       <c r="N16" t="str">
-        <v>10.112</v>
+        <v>22.000</v>
       </c>
       <c r="O16" t="str">
-        <v>9.685</v>
+        <v>18.408</v>
       </c>
       <c r="P16" t="str">
         <v>0</v>
@@ -1182,31 +1182,31 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>TQ-68</v>
+        <v>TQ-25</v>
       </c>
       <c r="B17" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C17" t="str">
-        <v>VIBRA PRESIDENTE PRUDENTE</v>
+        <v>VIBRA CUBATAO</v>
       </c>
       <c r="D17" t="str">
-        <v>0169/23F</v>
+        <v>0228/23</v>
       </c>
       <c r="E17" t="str">
-        <v>VIBRA CUB TRANSF CONF NF 1277460-0 14.09.23</v>
+        <v>NIMOFAST - ROMEOS - BL: 06 DENS: 0,8281</v>
       </c>
       <c r="F17" t="str">
-        <v>OLEO DIESEL S10</v>
+        <v>OLEO DIESEL S500</v>
       </c>
       <c r="G17" t="str">
-        <v>ONU 1202, DIESEL S10</v>
+        <v>ONU 1202, OLEO DIESEL S500</v>
       </c>
       <c r="H17" t="str">
-        <v>1.643</v>
+        <v>1.155.112</v>
       </c>
       <c r="I17" t="str">
-        <v>2.980</v>
+        <v>955.258</v>
       </c>
       <c r="J17" t="str">
         <v>0</v>
@@ -1221,10 +1221,10 @@
         <v>0</v>
       </c>
       <c r="N17" t="str">
-        <v>1.643</v>
+        <v>1.155.112</v>
       </c>
       <c r="O17" t="str">
-        <v>2.980</v>
+        <v>955.258</v>
       </c>
       <c r="P17" t="str">
         <v>0</v>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>TQ-68</v>
+        <v>TQ-29</v>
       </c>
       <c r="B18" t="str">
         <v>MERCADO INTERNO</v>
@@ -1241,22 +1241,22 @@
         <v>VIBRA CUBATAO</v>
       </c>
       <c r="D18" t="str">
-        <v>0169/23G</v>
+        <v>0228/23</v>
       </c>
       <c r="E18" t="str">
-        <v>VIBRA PRES TRANSF CONF NF 607274-0 26.09.2023</v>
+        <v>NIMOFAST - ROMEOS - BL: 06 DENS: 0,8281</v>
       </c>
       <c r="F18" t="str">
-        <v>OLEO DIESEL S10</v>
+        <v>OLEO DIESEL S500</v>
       </c>
       <c r="G18" t="str">
-        <v>ONU 1202, DIESEL S10</v>
+        <v>ONU 1202, OLEO DIESEL S500</v>
       </c>
       <c r="H18" t="str">
-        <v>20.556</v>
+        <v>578.249</v>
       </c>
       <c r="I18" t="str">
-        <v>17.730</v>
+        <v>478.202</v>
       </c>
       <c r="J18" t="str">
         <v>0</v>
@@ -1271,10 +1271,10 @@
         <v>0</v>
       </c>
       <c r="N18" t="str">
-        <v>20.556</v>
+        <v>578.249</v>
       </c>
       <c r="O18" t="str">
-        <v>17.730</v>
+        <v>478.202</v>
       </c>
       <c r="P18" t="str">
         <v>0</v>
@@ -1282,31 +1282,31 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>TQ-68</v>
+        <v>TQ-38</v>
       </c>
       <c r="B19" t="str">
-        <v>MERCADO INTERNO</v>
+        <v>IMPORTACAO COMUM</v>
       </c>
       <c r="C19" t="str">
         <v>VIBRA CUBATAO</v>
       </c>
       <c r="D19" t="str">
-        <v>0177/23B</v>
+        <v>0192/23A</v>
       </c>
       <c r="E19" t="str">
-        <v>TRANSF NIMOFAST X VIBRA CUB CONF NF 2217-1 09.10.23</v>
+        <v>TORM ATLANTIC - VIBRA CUBATÃO BL:05 - DENS:0,8305</v>
       </c>
       <c r="F19" t="str">
-        <v>OLEO DIESEL S10</v>
+        <v>OLEO DIESEL S500</v>
       </c>
       <c r="G19" t="str">
-        <v>OLEO DIESEL S10 ONU</v>
+        <v>ONU 1202, OLEO DIESEL S500</v>
       </c>
       <c r="H19" t="str">
-        <v>2.200</v>
+        <v>1.805</v>
       </c>
       <c r="I19" t="str">
-        <v>1.145</v>
+        <v>2.000</v>
       </c>
       <c r="J19" t="str">
         <v>0</v>
@@ -1321,10 +1321,10 @@
         <v>0</v>
       </c>
       <c r="N19" t="str">
-        <v>2.200</v>
+        <v>1.805</v>
       </c>
       <c r="O19" t="str">
-        <v>1.145</v>
+        <v>2.000</v>
       </c>
       <c r="P19" t="str">
         <v>0</v>
@@ -1332,31 +1332,31 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>TQ-68</v>
+        <v>TQ-38</v>
       </c>
       <c r="B20" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C20" t="str">
-        <v>VIBRA PAULINIA</v>
+        <v>VIBRA SAO PAULO</v>
       </c>
       <c r="D20" t="str">
-        <v>0177/23C</v>
+        <v>0192/23C</v>
       </c>
       <c r="E20" t="str">
-        <v>TRANSF  VIBRA CUB P/VIBRA PAULINIA CONF NF 1283140-0 DE09.10.23</v>
+        <v>TRANSF V.CUB X SP CONF NF 1285073-0 DENS:0,8298</v>
       </c>
       <c r="F20" t="str">
-        <v>OLEO DIESEL S10</v>
+        <v>OLEO DIESEL S500</v>
       </c>
       <c r="G20" t="str">
-        <v>OLEO DIESEL S10 ONU</v>
+        <v>ONU 1202, OLEO DIESEL S500</v>
       </c>
       <c r="H20" t="str">
-        <v>10.136</v>
+        <v>22.696</v>
       </c>
       <c r="I20" t="str">
-        <v>10.110</v>
+        <v>18.460</v>
       </c>
       <c r="J20" t="str">
         <v>0</v>
@@ -1371,10 +1371,10 @@
         <v>0</v>
       </c>
       <c r="N20" t="str">
-        <v>10.136</v>
+        <v>22.696</v>
       </c>
       <c r="O20" t="str">
-        <v>10.110</v>
+        <v>18.460</v>
       </c>
       <c r="P20" t="str">
         <v>0</v>
@@ -1382,31 +1382,31 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>TQ-68</v>
+        <v>TQ-38</v>
       </c>
       <c r="B21" t="str">
         <v>MERCADO INTERNO</v>
       </c>
       <c r="C21" t="str">
-        <v>VIBRA BARUERI</v>
+        <v>VIBRA RIBEIRAO PRETO</v>
       </c>
       <c r="D21" t="str">
-        <v>0177/23E</v>
+        <v>0192/23D</v>
       </c>
       <c r="E21" t="str">
-        <v>TRANSF  VIBRA CUB X VIBRA BARUERI CONF NF 1283141 09.10.23</v>
+        <v>TRANSF V.CUB X R.PRETO CONF NF 12470085-0 DENS:0,8298</v>
       </c>
       <c r="F21" t="str">
-        <v>OLEO DIESEL S10</v>
+        <v>OLEO DIESEL S500</v>
       </c>
       <c r="G21" t="str">
-        <v>OLEO DIESEL S10 ONU</v>
+        <v>ONU 1202, OLEO DIESEL S500</v>
       </c>
       <c r="H21" t="str">
-        <v>904.342</v>
+        <v>467.996</v>
       </c>
       <c r="I21" t="str">
-        <v>748.400</v>
+        <v>388.098</v>
       </c>
       <c r="J21" t="str">
         <v>0</v>
@@ -1421,10 +1421,10 @@
         <v>0</v>
       </c>
       <c r="N21" t="str">
-        <v>904.342</v>
+        <v>467.996</v>
       </c>
       <c r="O21" t="str">
-        <v>748.400</v>
+        <v>388.098</v>
       </c>
       <c r="P21" t="str">
         <v>0</v>
@@ -1432,42 +1432,192 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
+        <v>TQ-38</v>
+      </c>
+      <c r="B22" t="str">
+        <v>MERCADO INTERNO</v>
+      </c>
+      <c r="C22" t="str">
+        <v>VIBRA CUBATAO</v>
+      </c>
+      <c r="D22" t="str">
+        <v>0192/23E</v>
+      </c>
+      <c r="E22" t="str">
+        <v>TRANSF PAULINIA-CUBATAO CONF NF 3749230-1 DENS:0,8298</v>
+      </c>
+      <c r="F22" t="str">
+        <v>OLEO DIESEL S500</v>
+      </c>
+      <c r="G22" t="str">
+        <v>ONU 1202, OLEO DIESEL S500</v>
+      </c>
+      <c r="H22" t="str">
+        <v>10.112</v>
+      </c>
+      <c r="I22" t="str">
+        <v>9.685</v>
+      </c>
+      <c r="J22" t="str">
+        <v>0</v>
+      </c>
+      <c r="K22" t="str">
+        <v>0</v>
+      </c>
+      <c r="L22" t="str">
+        <v>0</v>
+      </c>
+      <c r="M22" t="str">
+        <v>0</v>
+      </c>
+      <c r="N22" t="str">
+        <v>10.112</v>
+      </c>
+      <c r="O22" t="str">
+        <v>9.685</v>
+      </c>
+      <c r="P22" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>TQ-43</v>
+      </c>
+      <c r="B23" t="str">
+        <v>MERCADO INTERNO</v>
+      </c>
+      <c r="C23" t="str">
+        <v>VIBRA CUBATAO</v>
+      </c>
+      <c r="D23" t="str">
+        <v>0228/23</v>
+      </c>
+      <c r="E23" t="str">
+        <v>NIMOFAST - ROMEOS - BL: 06 DENS: 0,8281</v>
+      </c>
+      <c r="F23" t="str">
+        <v>OLEO DIESEL S500</v>
+      </c>
+      <c r="G23" t="str">
+        <v>ONU 1202, OLEO DIESEL S500</v>
+      </c>
+      <c r="H23" t="str">
+        <v>2.008.248</v>
+      </c>
+      <c r="I23" t="str">
+        <v>1.660.788</v>
+      </c>
+      <c r="J23" t="str">
+        <v>0</v>
+      </c>
+      <c r="K23" t="str">
+        <v>0</v>
+      </c>
+      <c r="L23" t="str">
+        <v>0</v>
+      </c>
+      <c r="M23" t="str">
+        <v>0</v>
+      </c>
+      <c r="N23" t="str">
+        <v>2.008.248</v>
+      </c>
+      <c r="O23" t="str">
+        <v>1.660.788</v>
+      </c>
+      <c r="P23" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>TQ-59</v>
+      </c>
+      <c r="B24" t="str">
+        <v>MERCADO INTERNO</v>
+      </c>
+      <c r="C24" t="str">
+        <v>VIBRA CUBATAO</v>
+      </c>
+      <c r="D24" t="str">
+        <v>0228/23</v>
+      </c>
+      <c r="E24" t="str">
+        <v>NIMOFAST - ROMEOS - BL: 06 DENS: 0,8281</v>
+      </c>
+      <c r="F24" t="str">
+        <v>OLEO DIESEL S500</v>
+      </c>
+      <c r="G24" t="str">
+        <v>ONU 1202, OLEO DIESEL S500</v>
+      </c>
+      <c r="H24" t="str">
+        <v>1.253.530</v>
+      </c>
+      <c r="I24" t="str">
+        <v>1.036.649</v>
+      </c>
+      <c r="J24" t="str">
+        <v>0</v>
+      </c>
+      <c r="K24" t="str">
+        <v>0</v>
+      </c>
+      <c r="L24" t="str">
+        <v>0</v>
+      </c>
+      <c r="M24" t="str">
+        <v>0</v>
+      </c>
+      <c r="N24" t="str">
+        <v>1.253.530</v>
+      </c>
+      <c r="O24" t="str">
+        <v>1.036.649</v>
+      </c>
+      <c r="P24" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
         <v>Z</v>
       </c>
-      <c r="D22" t="str">
+      <c r="D25" t="str">
         <v>Total</v>
       </c>
-      <c r="H22" t="str">
-        <v>1.525.633</v>
-      </c>
-      <c r="I22" t="str">
-        <v>1.272.652</v>
-      </c>
-      <c r="J22" t="str">
-        <v>0</v>
-      </c>
-      <c r="K22" t="str">
-        <v>0</v>
-      </c>
-      <c r="L22" t="str">
-        <v>0</v>
-      </c>
-      <c r="M22" t="str">
-        <v>0</v>
-      </c>
-      <c r="N22" t="str">
-        <v>1.525.633</v>
-      </c>
-      <c r="O22" t="str">
-        <v>1.272.652</v>
-      </c>
-      <c r="P22" t="str">
+      <c r="H25" t="str">
+        <v>5.646.865</v>
+      </c>
+      <c r="I25" t="str">
+        <v>4.680.239</v>
+      </c>
+      <c r="J25" t="str">
+        <v>0</v>
+      </c>
+      <c r="K25" t="str">
+        <v>0</v>
+      </c>
+      <c r="L25" t="str">
+        <v>0</v>
+      </c>
+      <c r="M25" t="str">
+        <v>0</v>
+      </c>
+      <c r="N25" t="str">
+        <v>5.646.865</v>
+      </c>
+      <c r="O25" t="str">
+        <v>4.680.239</v>
+      </c>
+      <c r="P25" t="str">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:P22"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:P25"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>